<commit_message>
added myaccount page & registration page sc 2 and sc 3
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelData/storeIds.xlsx
+++ b/src/test/resources/ExcelData/storeIds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\durga\OneDrive\Desktop\Automation\BDD\ShopTestNG\src\test\resources\ExcelData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3F2CE6-7CBF-4536-AB66-7C7EAF0D2D7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{483095FB-B3D9-460E-AD5D-D957F8008917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{A0AC3805-2DF6-4E88-B53A-5AB6CB4933FE}"/>
+    <workbookView xWindow="3340" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{A0AC3805-2DF6-4E88-B53A-5AB6CB4933FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,15 +34,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>jEgFPF3LKv@gmail.com</t>
   </si>
   <si>
-    <t>Registered Email Id's</t>
-  </si>
-  <si>
     <t>MgXMUk5Brz@gmail.com</t>
+  </si>
+  <si>
+    <t>VsPxaWd40T@gmail.com</t>
+  </si>
+  <si>
+    <t>Registered_EmailIds</t>
+  </si>
+  <si>
+    <t>MiCcv4AjCP@gmail.com</t>
+  </si>
+  <si>
+    <t>SgQCS3JTB6@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -428,11 +437,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD7AFAA-887F-4738-954B-79AE62360462}">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -441,7 +448,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -449,9 +456,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s" s="0">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>